<commit_message>
Graphs and excel updated
</commit_message>
<xml_diff>
--- a/Outputs/ExperimentOutput.xlsx
+++ b/Outputs/ExperimentOutput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b1a534b4336b0e73/ASU Documents/ASU Year Five/Advanced Computer Networks/Project/Source/ACNFabricProject/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC104827515E72FE5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFDA4345-E408-4764-9510-14919A17AC6F}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="11_F25DC773A252ABDACC104827515E72FE5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A241E53-56BE-4346-8743-BA81E6B27429}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3525" yWindow="3525" windowWidth="21585" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Node</t>
   </si>
@@ -42,7 +42,10 @@
     <t>RTT</t>
   </si>
   <si>
-    <t>FR</t>
+    <t>Avg FR</t>
+  </si>
+  <si>
+    <t>Avg BW</t>
   </si>
 </sst>
 </file>
@@ -364,15 +367,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,62 +394,284 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1080</v>
       </c>
+      <c r="C2">
+        <v>8.33</v>
+      </c>
+      <c r="D2">
+        <v>0.32</v>
+      </c>
       <c r="F2">
-        <v>27.258359550561799</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>67.770475000000005</v>
+      </c>
+      <c r="G2">
+        <v>109.83050847457601</v>
+      </c>
+      <c r="H2">
+        <v>468.317288135593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>1080</v>
+      </c>
+      <c r="C3">
+        <v>16.66</v>
+      </c>
+      <c r="D3">
+        <v>0.64</v>
+      </c>
+      <c r="F3">
+        <v>93.222066666666606</v>
+      </c>
+      <c r="G3">
+        <v>57.745762711864401</v>
+      </c>
+      <c r="H3">
+        <v>246.227932203389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>720</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1080</v>
+      <c r="C4">
+        <v>8.33</v>
+      </c>
+      <c r="D4">
+        <v>0.32</v>
       </c>
       <c r="F4">
-        <v>79.674639999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68.371228915662599</v>
+      </c>
+      <c r="G4">
+        <v>110.186440677966</v>
+      </c>
+      <c r="H4">
+        <v>469.83498305084697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>720</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>16.66</v>
+      </c>
+      <c r="D5">
+        <v>0.64</v>
+      </c>
+      <c r="F5">
+        <v>91.800146341463403</v>
+      </c>
+      <c r="G5">
+        <v>57.711864406779597</v>
+      </c>
+      <c r="H5">
+        <v>246.083389830508</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>1080</v>
       </c>
+      <c r="C6">
+        <v>8.33</v>
+      </c>
+      <c r="D6">
+        <v>0.32</v>
+      </c>
       <c r="F6">
-        <v>113.108928571428</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120.027583333333</v>
+      </c>
+      <c r="G6">
+        <v>28.932203389830502</v>
+      </c>
+      <c r="H6">
+        <v>123.366915254237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1080</v>
+      </c>
+      <c r="C7">
+        <v>16.66</v>
+      </c>
+      <c r="D7">
+        <v>0.64</v>
+      </c>
+      <c r="F7">
+        <v>127.963130434782</v>
+      </c>
+      <c r="G7">
+        <v>28.677966101694899</v>
+      </c>
+      <c r="H7">
+        <v>122.282847457627</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>720</v>
+      </c>
+      <c r="C8">
+        <v>8.33</v>
+      </c>
+      <c r="D8">
+        <v>0.32</v>
+      </c>
+      <c r="F8">
+        <v>119.45613636363601</v>
+      </c>
+      <c r="G8">
+        <v>28.864406779661</v>
+      </c>
+      <c r="H8">
+        <v>123.07783050847399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>720</v>
+      </c>
+      <c r="C9">
+        <v>16.66</v>
+      </c>
+      <c r="D9">
+        <v>0.64</v>
+      </c>
+      <c r="F9">
+        <v>126.154368421052</v>
+      </c>
+      <c r="G9">
+        <v>28.745762711864401</v>
+      </c>
+      <c r="H9">
+        <v>122.571932203389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>3</v>
       </c>
-      <c r="B7">
+      <c r="B10">
+        <v>1080</v>
+      </c>
+      <c r="C10">
+        <v>8.33</v>
+      </c>
+      <c r="D10">
+        <v>0.32</v>
+      </c>
+      <c r="F10">
+        <v>149.988888888888</v>
+      </c>
+      <c r="G10">
+        <v>19.982758620689602</v>
+      </c>
+      <c r="H10">
+        <v>85.206482758620595</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>1080</v>
+      </c>
+      <c r="C11">
+        <v>16.66</v>
+      </c>
+      <c r="D11">
+        <v>0.64</v>
+      </c>
+      <c r="F11">
+        <v>161.73072727272699</v>
+      </c>
+      <c r="G11">
+        <v>19.982758620689602</v>
+      </c>
+      <c r="H11">
+        <v>85.206482758620595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
         <v>720</v>
+      </c>
+      <c r="C12">
+        <v>8.33</v>
+      </c>
+      <c r="D12">
+        <v>0.32</v>
+      </c>
+      <c r="F12">
+        <v>152.130764705882</v>
+      </c>
+      <c r="G12">
+        <v>19.982758620689602</v>
+      </c>
+      <c r="H12">
+        <v>85.206482758620595</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>720</v>
+      </c>
+      <c r="C13">
+        <v>16.66</v>
+      </c>
+      <c r="D13">
+        <v>0.64</v>
+      </c>
+      <c r="F13">
+        <v>155.1001</v>
+      </c>
+      <c r="G13">
+        <v>19.982758620689602</v>
+      </c>
+      <c r="H13">
+        <v>85.206482758620595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>